<commit_message>
860143 Test Mirror results
</commit_message>
<xml_diff>
--- a/Test/Build 6/ib_2_608 Test Mirror Log.xlsx
+++ b/Test/Build 6/ib_2_608 Test Mirror Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VACOAPVCPM1001.dva.va.gov\FolderRedirection$\DVA\vacoclarkj5\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MCCF PMO 2016\TAS FY16\eBilling\Build 5_6\IOC entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
   <si>
     <t>Comments</t>
   </si>
@@ -227,23 +227,23 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,7 +586,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,24 +601,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -643,43 +643,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="15" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <v>43409</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>43406</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="12">
         <v>43409</v>
       </c>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="1:7" s="15" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13" t="s">
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -801,7 +801,9 @@
       <c r="B11" s="8">
         <v>2599</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
@@ -816,7 +818,9 @@
       <c r="B12" s="8">
         <v>2599</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D12" s="8" t="s">
         <v>20</v>
       </c>
@@ -831,7 +835,9 @@
       <c r="B13" s="8">
         <v>2599</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
@@ -846,7 +852,9 @@
       <c r="B14" s="8">
         <v>2599</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D14" s="8" t="s">
         <v>20</v>
       </c>

</xml_diff>